<commit_message>
Updated first mature age to 2 (3 here cause first age is 1)
</commit_message>
<xml_diff>
--- a/data/hake220203.xlsx
+++ b/data/hake220203.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2A3528-B9F2-904E-A564-2F36C78861E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BB7221-5242-994E-9BE8-5BCB45107A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33620" yWindow="500" windowWidth="38400" windowHeight="42700" firstSheet="3" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="500" windowWidth="26340" windowHeight="20500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1960,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="B15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2910,7 +2910,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25297,8 +25297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25403,10 +25403,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -30440,14 +30440,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="175" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="6"/>
+    <col min="2" max="2" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -33564,7 +33564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:I401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G219" sqref="G219"/>
     </sheetView>
   </sheetViews>

</xml_diff>